<commit_message>
Adjust material in notes
</commit_message>
<xml_diff>
--- a/_Notes/Timetracking.xlsx
+++ b/_Notes/Timetracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\TUM\Bachelor Thesis\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\TUM\Bachelor Thesis\typing-tutor\_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50FB938-C93A-4FDA-9DD7-EA18C4ACD05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F351662-419D-4E62-A833-36F9A5406945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -784,6 +784,24 @@
         <v>14</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="2">
+        <v>44585</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" ref="D19" si="10">C19-B19</f>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>